<commit_message>
Adiciona arquivos com informações do plot do PLSR com filtro MSC
</commit_message>
<xml_diff>
--- a/Partial Least Squares Regression/plot_infos_plsr_msc.xlsx
+++ b/Partial Least Squares Regression/plot_infos_plsr_msc.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,22 +446,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>R²</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>RMSE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Offset</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Slope</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Offset</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>RMSE</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>R²</t>
         </is>
       </c>
     </row>
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.819933594090131</v>
+        <v>0.8199335940901312</v>
       </c>
       <c r="D2" t="n">
-        <v>2.520106522025432</v>
+        <v>1.127220969087652</v>
       </c>
       <c r="E2" t="n">
-        <v>1.127220969087652</v>
+        <v>2.520106522025437</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8199335940901312</v>
+        <v>0.8199335940901306</v>
       </c>
     </row>
     <row r="3">
@@ -501,40 +501,40 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7940417253792329</v>
+        <v>0.7346559650931279</v>
       </c>
       <c r="D3" t="n">
-        <v>2.888446474693272</v>
+        <v>1.368350563738811</v>
       </c>
       <c r="E3" t="n">
-        <v>1.36835056373881</v>
+        <v>2.888446474693278</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7346559650931281</v>
+        <v>0.7940417253792327</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>SST</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6194159694246291</v>
+        <v>0.7655841729998452</v>
       </c>
       <c r="D4" t="n">
-        <v>1.250035860105418</v>
+        <v>1.018845322461626</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1902692615977709</v>
+        <v>1.140579832143205</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6194159694246288</v>
+        <v>0.9184848592463797</v>
       </c>
     </row>
     <row r="5">
@@ -545,74 +545,74 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Predição</t>
+          <t>Referência</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5007262729700144</v>
+        <v>0.6194159694246284</v>
       </c>
       <c r="D5" t="n">
-        <v>1.638481421637806</v>
+        <v>0.190269261597771</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2345053188198085</v>
+        <v>1.250035860105419</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4218790728609438</v>
+        <v>0.6194159694246288</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Predição</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.6414071220225401</v>
+        <v>0.4218790728609437</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4026198869844522</v>
+        <v>0.2345053188198085</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3511647500287418</v>
+        <v>1.638481421637806</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6414071220225404</v>
+        <v>0.500726272970014</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Predição</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5332948426516068</v>
+        <v>0.266817439306803</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5280357467405117</v>
+        <v>0.2256539394122687</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4459264415167443</v>
+        <v>1.310329444091793</v>
       </c>
       <c r="F7" t="n">
-        <v>0.421762464562057</v>
+        <v>0.6113653378733529</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FIRMEZA (N)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -621,22 +621,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6496827478533524</v>
+        <v>0.6414071220225402</v>
       </c>
       <c r="D8" t="n">
-        <v>179.7162855527574</v>
+        <v>0.3511647500287419</v>
       </c>
       <c r="E8" t="n">
-        <v>60.82710683345289</v>
+        <v>0.4026198869844502</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6496827478533532</v>
+        <v>0.6414071220225416</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FIRMEZA (N)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -645,64 +645,184 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.5208172050466634</v>
+        <v>0.4217624645620563</v>
       </c>
       <c r="D9" t="n">
-        <v>245.1575041810687</v>
+        <v>0.4459264415167446</v>
       </c>
       <c r="E9" t="n">
-        <v>80.64238526564253</v>
+        <v>0.5280357467405109</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3842648662530816</v>
+        <v>0.5332948426516071</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UBS (%)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6474430404511623</v>
+        <v>0.686274151730107</v>
       </c>
       <c r="D10" t="n">
-        <v>5.407883862135074</v>
+        <v>0.244982744917667</v>
       </c>
       <c r="E10" t="n">
-        <v>1.910040297746731</v>
+        <v>-0.04118963980369106</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6474430404511629</v>
+        <v>0.9987623197514067</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Referência</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.6496827478533534</v>
+      </c>
+      <c r="D11" t="n">
+        <v>60.82710683345287</v>
+      </c>
+      <c r="E11" t="n">
+        <v>179.7162855527577</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6496827478533519</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Predição</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.384264866253081</v>
+      </c>
+      <c r="D12" t="n">
+        <v>80.64238526564257</v>
+      </c>
+      <c r="E12" t="n">
+        <v>245.1575041810685</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.5208172050466638</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Validação</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.5297024350879151</v>
+      </c>
+      <c r="D13" t="n">
+        <v>52.98044118784288</v>
+      </c>
+      <c r="E13" t="n">
+        <v>52.66918871666712</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.8818941314237686</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>UBS (%)</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Referência</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.6474430404511626</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.910040297746731</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5.407883862135076</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.6474430404511622</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>UBS (%)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Predição</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C15" t="n">
+        <v>0.5981015966807981</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.039323032879718</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5.813119203718665</v>
+      </c>
+      <c r="F15" t="n">
         <v>0.6206258724684867</v>
       </c>
-      <c r="D11" t="n">
-        <v>5.813119203718662</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2.039323032879718</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.5981015966807981</v>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UBS (%)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Validação</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.5953310123975417</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.378569044227535</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.397207338705432</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.787222122260882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza legenda na plotagem dos gráficos do PLSR
</commit_message>
<xml_diff>
--- a/Partial Least Squares Regression/plot_infos_plsr_msc.xlsx
+++ b/Partial Least Squares Regression/plot_infos_plsr_msc.xlsx
@@ -483,10 +483,10 @@
         <v>1.127220969087652</v>
       </c>
       <c r="E2" t="n">
-        <v>2.520106522025437</v>
+        <v>2.520106522025432</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8199335940901306</v>
+        <v>0.819933594090131</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7346559650931279</v>
+        <v>0.7346559650931281</v>
       </c>
       <c r="D3" t="n">
-        <v>1.368350563738811</v>
+        <v>1.36835056373881</v>
       </c>
       <c r="E3" t="n">
-        <v>2.888446474693278</v>
+        <v>2.888446474693272</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7940417253792327</v>
+        <v>0.7940417253792329</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.7655841729998452</v>
+        <v>0.7655841729998449</v>
       </c>
       <c r="D4" t="n">
         <v>1.018845322461626</v>
       </c>
       <c r="E4" t="n">
-        <v>1.140579832143205</v>
+        <v>1.140579832143217</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9184848592463797</v>
+        <v>0.918484859246379</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.6194159694246284</v>
+        <v>0.6194159694246288</v>
       </c>
       <c r="D5" t="n">
-        <v>0.190269261597771</v>
+        <v>0.1902692615977709</v>
       </c>
       <c r="E5" t="n">
-        <v>1.250035860105419</v>
+        <v>1.250035860105418</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6194159694246288</v>
+        <v>0.6194159694246291</v>
       </c>
     </row>
     <row r="6">
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4218790728609437</v>
+        <v>0.4218790728609438</v>
       </c>
       <c r="D6" t="n">
         <v>0.2345053188198085</v>
@@ -582,7 +582,7 @@
         <v>1.638481421637806</v>
       </c>
       <c r="F6" t="n">
-        <v>0.500726272970014</v>
+        <v>0.5007262729700144</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.266817439306803</v>
+        <v>0.2668174393068026</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2256539394122687</v>
+        <v>0.2256539394122688</v>
       </c>
       <c r="E7" t="n">
-        <v>1.310329444091793</v>
+        <v>1.310329444091794</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6113653378733529</v>
+        <v>0.6113653378733526</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6414071220225402</v>
+        <v>0.6414071220225404</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3511647500287419</v>
+        <v>0.3511647500287418</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4026198869844502</v>
+        <v>0.4026198869844522</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6414071220225416</v>
+        <v>0.6414071220225401</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4217624645620563</v>
+        <v>0.421762464562057</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4459264415167446</v>
+        <v>0.4459264415167443</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5280357467405109</v>
+        <v>0.5280357467405117</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5332948426516071</v>
+        <v>0.5332948426516068</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.686274151730107</v>
+        <v>0.6862741517301056</v>
       </c>
       <c r="D10" t="n">
-        <v>0.244982744917667</v>
+        <v>0.2449827449176675</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.04118963980369106</v>
+        <v>-0.04118963980369439</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9987623197514067</v>
+        <v>0.9987623197514096</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6496827478533534</v>
+        <v>0.6496827478533532</v>
       </c>
       <c r="D11" t="n">
-        <v>60.82710683345287</v>
+        <v>60.82710683345289</v>
       </c>
       <c r="E11" t="n">
-        <v>179.7162855527577</v>
+        <v>179.7162855527574</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6496827478533519</v>
+        <v>0.6496827478533524</v>
       </c>
     </row>
     <row r="12">
@@ -717,16 +717,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.384264866253081</v>
+        <v>0.3842648662530816</v>
       </c>
       <c r="D12" t="n">
-        <v>80.64238526564257</v>
+        <v>80.64238526564253</v>
       </c>
       <c r="E12" t="n">
-        <v>245.1575041810685</v>
+        <v>245.1575041810687</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5208172050466638</v>
+        <v>0.5208172050466634</v>
       </c>
     </row>
     <row r="13">
@@ -744,13 +744,13 @@
         <v>0.5297024350879151</v>
       </c>
       <c r="D13" t="n">
-        <v>52.98044118784288</v>
+        <v>52.98044118784289</v>
       </c>
       <c r="E13" t="n">
-        <v>52.66918871666712</v>
+        <v>52.66918871666735</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8818941314237686</v>
+        <v>0.8818941314237679</v>
       </c>
     </row>
     <row r="14">
@@ -765,16 +765,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.6474430404511626</v>
+        <v>0.6474430404511629</v>
       </c>
       <c r="D14" t="n">
         <v>1.910040297746731</v>
       </c>
       <c r="E14" t="n">
-        <v>5.407883862135076</v>
+        <v>5.407883862135074</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6474430404511622</v>
+        <v>0.6474430404511623</v>
       </c>
     </row>
     <row r="15">
@@ -795,7 +795,7 @@
         <v>2.039323032879718</v>
       </c>
       <c r="E15" t="n">
-        <v>5.813119203718665</v>
+        <v>5.813119203718662</v>
       </c>
       <c r="F15" t="n">
         <v>0.6206258724684867</v>
@@ -813,16 +813,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.5953310123975417</v>
+        <v>0.5953310123975422</v>
       </c>
       <c r="D16" t="n">
-        <v>1.378569044227535</v>
+        <v>1.378569044227534</v>
       </c>
       <c r="E16" t="n">
-        <v>3.397207338705432</v>
+        <v>3.39720733870543</v>
       </c>
       <c r="F16" t="n">
-        <v>0.787222122260882</v>
+        <v>0.7872221222608822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>